<commit_message>
excel work full done
</commit_message>
<xml_diff>
--- a/src/main/java/com/smsa/backend/assets/testFile.xlsx
+++ b/src/main/java/com/smsa/backend/assets/testFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="79">
   <si>
     <t>Invoice#</t>
   </si>
@@ -146,6 +146,111 @@
   </si>
   <si>
     <t>System</t>
+  </si>
+  <si>
+    <t>muraza</t>
+  </si>
+  <si>
+    <t>2023-07-28</t>
+  </si>
+  <si>
+    <t>14146857414</t>
+  </si>
+  <si>
+    <t>RX6693</t>
+  </si>
+  <si>
+    <t>290407068985</t>
+  </si>
+  <si>
+    <t>LZ#1880-SA</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>Alhanouf Alsubaie</t>
+  </si>
+  <si>
+    <t>290407068996</t>
+  </si>
+  <si>
+    <t>LZ#1918-SA</t>
+  </si>
+  <si>
+    <t>Aisha Alqahtani</t>
+  </si>
+  <si>
+    <t>290407069003</t>
+  </si>
+  <si>
+    <t>LZ#2001-SA</t>
+  </si>
+  <si>
+    <t>Ebtehal Mm</t>
+  </si>
+  <si>
+    <t>290407069014</t>
+  </si>
+  <si>
+    <t>LZ#2004-SA</t>
+  </si>
+  <si>
+    <t>hala alwaely</t>
+  </si>
+  <si>
+    <t>290407069025</t>
+  </si>
+  <si>
+    <t>LZ#2005-SA</t>
+  </si>
+  <si>
+    <t>Elham Mohammed</t>
+  </si>
+  <si>
+    <t>290407069036</t>
+  </si>
+  <si>
+    <t>LZ#2010-SA</t>
+  </si>
+  <si>
+    <t>JAMALAH AL GAMDY</t>
+  </si>
+  <si>
+    <t>290407069047</t>
+  </si>
+  <si>
+    <t>LZ#1980-SA</t>
+  </si>
+  <si>
+    <t>عبدالرهاب المطرفي</t>
+  </si>
+  <si>
+    <t>290407069058</t>
+  </si>
+  <si>
+    <t>LZ#1974-SA</t>
+  </si>
+  <si>
+    <t>Afrah Alharbi</t>
+  </si>
+  <si>
+    <t>290407069069</t>
+  </si>
+  <si>
+    <t>LZ#1927-SA</t>
+  </si>
+  <si>
+    <t>Lolwah Ahmed</t>
+  </si>
+  <si>
+    <t>2023-07-29</t>
+  </si>
+  <si>
+    <t>dummy</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -338,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -410,6 +515,15 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="6" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
       <alignment horizontal="center"/>
     </xf>
@@ -663,18 +777,18 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.86" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="17.71" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="16.71" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="14.29" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="15.43" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="11.71" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="14.43" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="14.29" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="12.43" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="6.14" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="13.71" collapsed="false"/>
-    <col min="12" max="26" customWidth="true" width="8.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="14.86" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.71" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.71" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.29" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.43" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.71" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.43" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.29" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.43" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="6.14" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.71" collapsed="true"/>
+    <col min="12" max="26" customWidth="true" width="8.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -706,13 +820,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>45134.0</v>
+        <v>45136.0</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1"/>
@@ -751,18 +865,40 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="11"/>
@@ -1819,26 +1955,26 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.14" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.29" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="14.29" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="13.14" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="12.14" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="5.71" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="10.14" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="18.29" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="17.57" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="7.71" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="14.14" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="14.29" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="12.0" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="19.57" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="6.71" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="12.71" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" width="17.71" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="5.71" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="17.0" collapsed="false"/>
-    <col min="20" max="26" customWidth="true" width="8.71" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="13.14" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.29" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.29" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.14" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.14" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="5.71" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.14" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.29" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.57" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="7.71" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.14" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.29" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="19.57" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="6.71" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="12.71" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="17.71" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="5.71" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="20" max="26" customWidth="true" width="8.71" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -1900,24 +2036,24 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" s="29" customFormat="true">
+    <row r="2" s="32" customFormat="true">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
         <v>38</v>
@@ -1926,7 +2062,7 @@
         <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J2" t="s">
         <v>41</v>
@@ -1935,10 +2071,10 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>900.0</v>
+        <v>10.0</v>
       </c>
       <c r="M2" t="n">
-        <v>135.0</v>
+        <v>1.5</v>
       </c>
       <c r="N2" t="n">
         <v>0.0</v>
@@ -1947,182 +2083,462 @@
         <v>0.0</v>
       </c>
       <c r="P2" t="n">
-        <v>135.0</v>
+        <v>1.5</v>
       </c>
       <c r="Q2" t="n">
         <v>0.0</v>
       </c>
       <c r="R2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="20"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="20"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="20"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" s="32" customFormat="true">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" s="32" customFormat="true">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" s="32" customFormat="true">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" s="32" customFormat="true">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" s="32" customFormat="true">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" s="32" customFormat="true">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" s="32" customFormat="true">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" s="32" customFormat="true">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R10" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="20"/>

</xml_diff>

<commit_message>
so much work update
</commit_message>
<xml_diff>
--- a/src/main/java/com/smsa/backend/assets/testFile.xlsx
+++ b/src/main/java/com/smsa/backend/assets/testFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="101">
   <si>
     <t>Invoice#</t>
   </si>
@@ -251,6 +251,72 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>PAK</t>
+  </si>
+  <si>
+    <t>2023-07-31</t>
+  </si>
+  <si>
+    <t>14146857413</t>
+  </si>
+  <si>
+    <t>Murtaza</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>1454.0</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>242.0</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>2452.0</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>25.0</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>21.0</t>
+  </si>
+  <si>
+    <t>34.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>222.0</t>
   </si>
 </sst>
 </file>
@@ -443,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -515,6 +581,24 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="6" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
       <alignment horizontal="center"/>
     </xf>
@@ -809,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>4</v>
@@ -826,7 +910,7 @@
         <v>6</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>45136.0</v>
+        <v>45138.0</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1"/>
@@ -870,48 +954,70 @@
         <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="E10" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
       <c r="F10" t="n">
-        <v>3.0</v>
+        <v>640.5</v>
       </c>
       <c r="G10" t="n">
-        <v>90.0</v>
+        <v>50.0</v>
       </c>
       <c r="H10" t="n">
-        <v>13.5</v>
+        <v>7.5</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0</v>
+        <v>535.0</v>
       </c>
       <c r="J10" t="n">
         <v>0.0</v>
       </c>
       <c r="K10" t="n">
+        <v>535.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4847.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>4683.0</v>
+      </c>
+      <c r="J11" t="n">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
+      <c r="K11" t="n">
+        <v>4683.0</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="11"/>
@@ -2036,7 +2142,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" s="32" customFormat="true">
+    <row r="2" s="38" customFormat="true">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -2047,52 +2153,52 @@
         <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="H2" t="s">
         <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>10.0</v>
+        <v>85</v>
+      </c>
+      <c r="K2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" t="s">
+        <v>87</v>
       </c>
       <c r="M2" t="n">
         <v>1.5</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" t="n">
         <v>0.0</v>
       </c>
-      <c r="O2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1.5</v>
-      </c>
       <c r="Q2" t="n">
-        <v>0.0</v>
+        <v>1234.0</v>
       </c>
       <c r="R2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" s="32" customFormat="true">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" s="38" customFormat="true">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -2103,52 +2209,52 @@
         <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
         <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>10.0</v>
+        <v>85</v>
+      </c>
+      <c r="K3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" t="s">
+        <v>87</v>
       </c>
       <c r="M3" t="n">
         <v>1.5</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N3" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P3" t="n">
         <v>0.0</v>
       </c>
-      <c r="O3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1.5</v>
-      </c>
       <c r="Q3" t="n">
-        <v>0.0</v>
+        <v>1234.0</v>
       </c>
       <c r="R3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" s="32" customFormat="true">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" s="38" customFormat="true">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -2159,54 +2265,54 @@
         <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="H4" t="s">
         <v>39</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>10.0</v>
+        <v>85</v>
+      </c>
+      <c r="K4" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" t="s">
+        <v>87</v>
       </c>
       <c r="M4" t="n">
         <v>1.5</v>
       </c>
-      <c r="N4" t="n">
+      <c r="N4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P4" t="n">
         <v>0.0</v>
       </c>
-      <c r="O4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>1.5</v>
-      </c>
       <c r="Q4" t="n">
-        <v>0.0</v>
+        <v>1234.0</v>
       </c>
       <c r="R4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" s="32" customFormat="true">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" s="38" customFormat="true">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
@@ -2215,54 +2321,54 @@
         <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>10.0</v>
+        <v>85</v>
+      </c>
+      <c r="K5" t="s">
+        <v>94</v>
+      </c>
+      <c r="L5" t="s">
+        <v>87</v>
       </c>
       <c r="M5" t="n">
         <v>1.5</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N5" t="s">
+        <v>95</v>
+      </c>
+      <c r="O5" t="s">
+        <v>89</v>
+      </c>
+      <c r="P5" t="n">
         <v>0.0</v>
       </c>
-      <c r="O5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>1.5</v>
-      </c>
       <c r="Q5" t="n">
-        <v>0.0</v>
+        <v>3244.0</v>
       </c>
       <c r="R5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" s="32" customFormat="true">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" s="38" customFormat="true">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
@@ -2271,54 +2377,54 @@
         <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s">
         <v>39</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>10.0</v>
+        <v>85</v>
+      </c>
+      <c r="K6" t="s">
+        <v>96</v>
+      </c>
+      <c r="L6" t="s">
+        <v>87</v>
       </c>
       <c r="M6" t="n">
         <v>1.5</v>
       </c>
-      <c r="N6" t="n">
+      <c r="N6" t="s">
+        <v>97</v>
+      </c>
+      <c r="O6" t="s">
+        <v>89</v>
+      </c>
+      <c r="P6" t="n">
         <v>0.0</v>
       </c>
-      <c r="O6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>1.5</v>
-      </c>
       <c r="Q6" t="n">
-        <v>0.0</v>
+        <v>6366.0</v>
       </c>
       <c r="R6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" s="32" customFormat="true">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" s="38" customFormat="true">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -2327,54 +2433,54 @@
         <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
         <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>10.0</v>
+        <v>85</v>
+      </c>
+      <c r="K7" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" t="s">
+        <v>87</v>
       </c>
       <c r="M7" t="n">
         <v>1.5</v>
       </c>
-      <c r="N7" t="n">
+      <c r="N7" t="s">
+        <v>91</v>
+      </c>
+      <c r="O7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P7" t="n">
         <v>0.0</v>
       </c>
-      <c r="O7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>1.5</v>
-      </c>
       <c r="Q7" t="n">
-        <v>0.0</v>
+        <v>2335.0</v>
       </c>
       <c r="R7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" s="32" customFormat="true">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" s="38" customFormat="true">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
@@ -2383,54 +2489,54 @@
         <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="H8" t="s">
         <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>10.0</v>
+        <v>85</v>
+      </c>
+      <c r="K8" t="s">
+        <v>99</v>
+      </c>
+      <c r="L8" t="s">
+        <v>87</v>
       </c>
       <c r="M8" t="n">
         <v>1.5</v>
       </c>
-      <c r="N8" t="n">
+      <c r="N8" t="s">
+        <v>100</v>
+      </c>
+      <c r="O8" t="s">
+        <v>89</v>
+      </c>
+      <c r="P8" t="n">
         <v>0.0</v>
       </c>
-      <c r="O8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>1.5</v>
-      </c>
       <c r="Q8" t="n">
-        <v>0.0</v>
+        <v>51421.0</v>
       </c>
       <c r="R8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" s="32" customFormat="true">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" s="38" customFormat="true">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -2439,49 +2545,49 @@
         <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="H9" t="s">
         <v>39</v>
       </c>
       <c r="I9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>10.0</v>
+        <v>85</v>
+      </c>
+      <c r="K9" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" t="s">
+        <v>87</v>
       </c>
       <c r="M9" t="n">
         <v>1.5</v>
       </c>
-      <c r="N9" t="n">
+      <c r="N9" t="s">
+        <v>95</v>
+      </c>
+      <c r="O9" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" t="n">
         <v>0.0</v>
       </c>
-      <c r="O9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>1.5</v>
-      </c>
       <c r="Q9" t="n">
-        <v>0.0</v>
+        <v>14114.0</v>
       </c>
       <c r="R9" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" s="32" customFormat="true">

</xml_diff>